<commit_message>
tests added, api test sheet edited
</commit_message>
<xml_diff>
--- a/Report things/API_table.xlsx
+++ b/Report things/API_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB60DC4-A76A-465D-81B0-8B455C439EE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2617C4-10DE-45AD-B1D6-8A58C032E019}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,10 +414,6 @@
 2) Check that a response of type list is received </t>
   </si>
   <si>
-    <t>1) admin_id blank
-2) request_id blank</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) _id blank (generic error). More front end side since backend generates the id 
 </t>
   </si>
@@ -780,6 +776,11 @@
     <t xml:space="preserve">1) Valid admin_id sent 
 Check that a response of type list is received. Compare the date of the individual requests in the list  
 2) valid user_id sent. Check that a response of type list is received. Compare the date of the individual requests in the list  </t>
+  </si>
+  <si>
+    <t>1) admin_id blank
+2) request_id blank
+3) admin_id cant be found</t>
   </si>
 </sst>
 </file>
@@ -921,6 +922,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -931,12 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,7 +1279,7 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1296,7 +1297,7 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1314,7 +1315,7 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1332,7 +1333,7 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1376,7 +1377,7 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E12" s="1"/>
@@ -1392,13 +1393,13 @@
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="10" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1412,11 +1413,11 @@
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1428,11 +1429,11 @@
       <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1444,11 +1445,11 @@
       <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1460,11 +1461,11 @@
       <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1476,11 +1477,11 @@
       <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1492,11 +1493,11 @@
       <c r="C19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1508,11 +1509,11 @@
       <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1524,11 +1525,11 @@
       <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1540,11 +1541,11 @@
       <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1556,11 +1557,11 @@
       <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1572,11 +1573,11 @@
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1591,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D5DE48-BDB6-4AA5-AFF6-693BCA48552F}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="82" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,13 +1627,13 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1640,41 +1641,41 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>91</v>
+      <c r="D4" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1702,7 +1703,7 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1716,168 +1717,168 @@
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>93</v>
+      <c r="D11" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>94</v>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Copy the backend_new code
</commit_message>
<xml_diff>
--- a/Report things/API_table.xlsx
+++ b/Report things/API_table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2617C4-10DE-45AD-B1D6-8A58C032E019}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C834E14C-6071-411F-80A5-5AEB564FCE67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API LIST" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Case documentation" sheetId="2" r:id="rId2"/>
+    <sheet name="Request APIs" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Case documentation" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>Server URL</t>
   </si>
@@ -182,9 +183,6 @@
   </si>
   <si>
     <t>REQUESTS</t>
-  </si>
-  <si>
-    <t>Get user credentials from USERMANAGEMENT collection</t>
   </si>
   <si>
     <t>1) admin_id: String
@@ -781,6 +779,36 @@
     <t>1) admin_id blank
 2) request_id blank
 3) admin_id cant be found</t>
+  </si>
+  <si>
+    <t>Token is the user session object ID. This is used to search for specific UserObject ID.which then returns the username and is used in specific queries since requests are mapped to a user/admin's username</t>
+  </si>
+  <si>
+    <t>For admins to click on a button which assoicates a request to them. Essentially for them to take up a case. At the same time, this updates the notifications field of all team members and the user which is displayed upon login</t>
+  </si>
+  <si>
+    <t>/user/changepassword</t>
+  </si>
+  <si>
+    <t>/user/changeusername</t>
+  </si>
+  <si>
+    <t>/user/changeemail</t>
+  </si>
+  <si>
+    <t>/user/team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) token: String 
+2) Old Password: String
+3) New Password: String </t>
+  </si>
+  <si>
+    <t>1) token: String 
+2) new username: String</t>
+  </si>
+  <si>
+    <t>For clients and admins who want to change password</t>
   </si>
 </sst>
 </file>
@@ -911,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -938,6 +966,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1221,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
@@ -1280,7 +1312,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -1292,13 +1324,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -1316,7 +1348,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -1334,266 +1366,329 @@
         <v>19</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="86.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C5283-E6C2-4158-A1E2-080D1D150AC5}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
+    <col min="6" max="6" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="12"/>
+      <c r="F15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E13:E24"/>
-    <mergeCell ref="F13:F24"/>
+    <mergeCell ref="E4:E15"/>
+    <mergeCell ref="F4:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D5DE48-BDB6-4AA5-AFF6-693BCA48552F}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D22"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,13 +1709,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1628,13 +1723,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="216" x14ac:dyDescent="0.3">
@@ -1642,13 +1737,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
@@ -1656,13 +1751,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1670,13 +1765,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1690,13 +1785,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1704,13 +1799,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -1718,13 +1813,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -1732,13 +1827,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1746,13 +1841,13 @@
         <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1760,13 +1855,13 @@
         <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1774,13 +1869,13 @@
         <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -1788,13 +1883,13 @@
         <v>27</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1802,13 +1897,13 @@
         <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -1816,13 +1911,13 @@
         <v>29</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -1830,13 +1925,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -1844,13 +1939,13 @@
         <v>31</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -1858,13 +1953,13 @@
         <v>32</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -1872,13 +1967,13 @@
         <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>